<commit_message>
Updates on dashboard scripts, .gitignore, files, etc.
</commit_message>
<xml_diff>
--- a/Data/Ubicaciones/lista.xlsx
+++ b/Data/Ubicaciones/lista.xlsx
@@ -445,7 +445,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -530,6 +530,22 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,16 +599,16 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G25" activeCellId="0" sqref="G25"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="10.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="23.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="3" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="7.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.43"/>
@@ -1629,40 +1645,40 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="21" t="n">
         <v>100092</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="G28" s="3" t="n">
+      <c r="G28" s="23" t="n">
         <v>-6.92511</v>
       </c>
-      <c r="H28" s="3" t="n">
+      <c r="H28" s="23" t="n">
         <v>-79.12902</v>
       </c>
-      <c r="I28" s="4" t="n">
+      <c r="I28" s="24" t="n">
         <v>2424</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K28" s="4" t="n">
+      <c r="K28" s="24" t="n">
         <v>0</v>
       </c>
-      <c r="L28" s="4" t="n">
+      <c r="L28" s="24" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>